<commit_message>
Added TCP and RAM Configuration to InstallChecklist
</commit_message>
<xml_diff>
--- a/8. Harmonising standards/01_Project organisation/03_Project Documentation/Template Project Documentation 1.1.xlsx
+++ b/8. Harmonising standards/01_Project organisation/03_Project Documentation/Template Project Documentation 1.1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AB9FA2-5A3D-4126-BE3C-A12FB7609835}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC62AC4E-2C17-4278-82A6-B891D46E1533}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="4725" tabRatio="837" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="4725" tabRatio="837" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht" sheetId="47" r:id="rId1"/>
@@ -24,17 +24,22 @@
     <definedName name="spProfitLoss_Materialize_Control">Sample_PrzVerzeichnis!$A$25</definedName>
     <definedName name="spProfitLoss_Materialize_Structure">Sample_PrzVerzeichnis!$A$38</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="194">
   <si>
     <t>Corporate Design</t>
   </si>
@@ -702,6 +707,18 @@
   </si>
   <si>
     <t>Objektvorlagen im Corporate Design</t>
+  </si>
+  <si>
+    <t>TCP IP aktivieren</t>
+  </si>
+  <si>
+    <t>im SQL Server Konfigurationsmanager aktivieren</t>
+  </si>
+  <si>
+    <t>SQL Server RAM Einstellung prüfen</t>
+  </si>
+  <si>
+    <t>RAM Nutzung des SQL Servers auf ca. 2/3 der Server RAM begrenzen</t>
   </si>
 </sst>
 </file>
@@ -31147,7 +31164,7 @@
   </sheetPr>
   <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I33" sqref="I33"/>
     </sheetView>
@@ -33741,12 +33758,12 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:N1121"/>
+  <dimension ref="A1:N1123"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H33" sqref="H33"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34141,13 +34158,13 @@
       <c r="A20" s="99"/>
       <c r="B20" s="92"/>
       <c r="C20" s="41" t="s">
-        <v>122</v>
+        <v>190</v>
       </c>
       <c r="D20" s="94" t="s">
         <v>99</v>
       </c>
       <c r="E20" s="94" t="s">
-        <v>126</v>
+        <v>191</v>
       </c>
       <c r="F20" s="41"/>
       <c r="G20" s="137"/>
@@ -34160,34 +34177,40 @@
       <c r="M20" s="103"/>
       <c r="N20" s="103"/>
     </row>
-    <row r="21" spans="1:14" s="124" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="123"/>
-      <c r="B21" s="135" t="s">
-        <v>127</v>
+    <row r="21" spans="1:14" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="99"/>
+      <c r="B21" s="92"/>
+      <c r="C21" s="41" t="s">
+        <v>192</v>
       </c>
-      <c r="C21" s="136"/>
-      <c r="D21" s="126"/>
-      <c r="E21" s="127"/>
-      <c r="F21" s="127"/>
-      <c r="G21" s="138"/>
-      <c r="H21" s="129"/>
-      <c r="J21" s="125"/>
-      <c r="K21" s="125"/>
-      <c r="L21" s="125"/>
-      <c r="M21" s="125"/>
-      <c r="N21" s="125"/>
+      <c r="D21" s="94" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" s="94" t="s">
+        <v>193</v>
+      </c>
+      <c r="F21" s="41"/>
+      <c r="G21" s="137"/>
+      <c r="H21" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="J21" s="103"/>
+      <c r="K21" s="103"/>
+      <c r="L21" s="103"/>
+      <c r="M21" s="103"/>
+      <c r="N21" s="103"/>
     </row>
     <row r="22" spans="1:14" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="99"/>
       <c r="B22" s="92"/>
       <c r="C22" s="41" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D22" s="94" t="s">
         <v>99</v>
       </c>
       <c r="E22" s="94" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F22" s="41"/>
       <c r="G22" s="137"/>
@@ -34200,38 +34223,34 @@
       <c r="M22" s="103"/>
       <c r="N22" s="103"/>
     </row>
-    <row r="23" spans="1:14" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="99"/>
-      <c r="B23" s="92"/>
-      <c r="C23" s="41" t="s">
-        <v>130</v>
+    <row r="23" spans="1:14" s="124" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="123"/>
+      <c r="B23" s="135" t="s">
+        <v>127</v>
       </c>
-      <c r="D23" s="94" t="s">
-        <v>99</v>
-      </c>
-      <c r="E23" s="94"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="137"/>
-      <c r="H23" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="J23" s="103"/>
-      <c r="K23" s="103"/>
-      <c r="L23" s="103"/>
-      <c r="M23" s="103"/>
-      <c r="N23" s="103"/>
+      <c r="C23" s="136"/>
+      <c r="D23" s="126"/>
+      <c r="E23" s="127"/>
+      <c r="F23" s="127"/>
+      <c r="G23" s="138"/>
+      <c r="H23" s="129"/>
+      <c r="J23" s="125"/>
+      <c r="K23" s="125"/>
+      <c r="L23" s="125"/>
+      <c r="M23" s="125"/>
+      <c r="N23" s="125"/>
     </row>
     <row r="24" spans="1:14" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="99"/>
       <c r="B24" s="92"/>
       <c r="C24" s="41" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D24" s="94" t="s">
         <v>99</v>
       </c>
       <c r="E24" s="94" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F24" s="41"/>
       <c r="G24" s="137"/>
@@ -34248,14 +34267,12 @@
       <c r="A25" s="99"/>
       <c r="B25" s="92"/>
       <c r="C25" s="41" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D25" s="94" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
-      <c r="E25" s="94" t="s">
-        <v>135</v>
-      </c>
+      <c r="E25" s="94"/>
       <c r="F25" s="41"/>
       <c r="G25" s="137"/>
       <c r="H25" s="42" t="s">
@@ -34271,13 +34288,13 @@
       <c r="A26" s="99"/>
       <c r="B26" s="92"/>
       <c r="C26" s="41" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D26" s="94" t="s">
         <v>99</v>
       </c>
       <c r="E26" s="94" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F26" s="41"/>
       <c r="G26" s="137"/>
@@ -34290,21 +34307,21 @@
       <c r="M26" s="103"/>
       <c r="N26" s="103"/>
     </row>
-    <row r="27" spans="1:14" s="37" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="99"/>
       <c r="B27" s="92"/>
-      <c r="C27" s="120" t="s">
-        <v>142</v>
+      <c r="C27" s="41" t="s">
+        <v>134</v>
       </c>
-      <c r="D27" s="121" t="s">
-        <v>99</v>
+      <c r="D27" s="94" t="s">
+        <v>117</v>
       </c>
-      <c r="E27" s="121" t="s">
-        <v>143</v>
+      <c r="E27" s="94" t="s">
+        <v>135</v>
       </c>
-      <c r="F27" s="120"/>
-      <c r="G27" s="140"/>
-      <c r="H27" s="122" t="s">
+      <c r="F27" s="41"/>
+      <c r="G27" s="137"/>
+      <c r="H27" s="42" t="s">
         <v>46</v>
       </c>
       <c r="J27" s="103"/>
@@ -34316,20 +34333,18 @@
     <row r="28" spans="1:14" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="99"/>
       <c r="B28" s="92"/>
-      <c r="C28" s="120" t="s">
-        <v>144</v>
+      <c r="C28" s="41" t="s">
+        <v>136</v>
       </c>
-      <c r="D28" s="121" t="s">
+      <c r="D28" s="94" t="s">
         <v>99</v>
       </c>
-      <c r="E28" s="121" t="s">
-        <v>176</v>
+      <c r="E28" s="94" t="s">
+        <v>137</v>
       </c>
-      <c r="F28" s="120"/>
-      <c r="G28" s="140" t="s">
-        <v>177</v>
-      </c>
-      <c r="H28" s="122" t="s">
+      <c r="F28" s="41"/>
+      <c r="G28" s="137"/>
+      <c r="H28" s="42" t="s">
         <v>46</v>
       </c>
       <c r="J28" s="103"/>
@@ -34338,38 +34353,46 @@
       <c r="M28" s="103"/>
       <c r="N28" s="103"/>
     </row>
-    <row r="29" spans="1:14" s="124" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="123"/>
-      <c r="B29" s="135" t="s">
-        <v>170</v>
+    <row r="29" spans="1:14" s="37" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="99"/>
+      <c r="B29" s="92"/>
+      <c r="C29" s="120" t="s">
+        <v>142</v>
       </c>
-      <c r="C29" s="136"/>
-      <c r="D29" s="126"/>
-      <c r="E29" s="127"/>
-      <c r="F29" s="127"/>
-      <c r="G29" s="138"/>
-      <c r="H29" s="129"/>
-      <c r="J29" s="125"/>
-      <c r="K29" s="125"/>
-      <c r="L29" s="125"/>
-      <c r="M29" s="125"/>
-      <c r="N29" s="125"/>
-    </row>
-    <row r="30" spans="1:14" s="37" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="D29" s="121" t="s">
+        <v>99</v>
+      </c>
+      <c r="E29" s="121" t="s">
+        <v>143</v>
+      </c>
+      <c r="F29" s="120"/>
+      <c r="G29" s="140"/>
+      <c r="H29" s="122" t="s">
+        <v>46</v>
+      </c>
+      <c r="J29" s="103"/>
+      <c r="K29" s="103"/>
+      <c r="L29" s="103"/>
+      <c r="M29" s="103"/>
+      <c r="N29" s="103"/>
+    </row>
+    <row r="30" spans="1:14" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="99"/>
       <c r="B30" s="92"/>
-      <c r="C30" s="41" t="s">
-        <v>42</v>
+      <c r="C30" s="120" t="s">
+        <v>144</v>
       </c>
-      <c r="D30" s="94" t="s">
+      <c r="D30" s="121" t="s">
         <v>99</v>
       </c>
-      <c r="E30" s="94" t="s">
-        <v>156</v>
+      <c r="E30" s="121" t="s">
+        <v>176</v>
       </c>
-      <c r="F30" s="41"/>
-      <c r="G30" s="137"/>
-      <c r="H30" s="42" t="s">
+      <c r="F30" s="120"/>
+      <c r="G30" s="140" t="s">
+        <v>177</v>
+      </c>
+      <c r="H30" s="122" t="s">
         <v>46</v>
       </c>
       <c r="J30" s="103"/>
@@ -34378,40 +34401,34 @@
       <c r="M30" s="103"/>
       <c r="N30" s="103"/>
     </row>
-    <row r="31" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="99"/>
-      <c r="B31" s="92"/>
-      <c r="C31" s="41" t="s">
-        <v>159</v>
+    <row r="31" spans="1:14" s="124" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="123"/>
+      <c r="B31" s="135" t="s">
+        <v>170</v>
       </c>
-      <c r="D31" s="94" t="s">
-        <v>99</v>
-      </c>
-      <c r="E31" s="94" t="s">
-        <v>158</v>
-      </c>
-      <c r="F31" s="41"/>
-      <c r="G31" s="137"/>
-      <c r="H31" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="J31" s="103"/>
-      <c r="K31" s="103"/>
-      <c r="L31" s="103"/>
-      <c r="M31" s="103"/>
-      <c r="N31" s="103"/>
-    </row>
-    <row r="32" spans="1:14" s="37" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="100"/>
+      <c r="C31" s="136"/>
+      <c r="D31" s="126"/>
+      <c r="E31" s="127"/>
+      <c r="F31" s="127"/>
+      <c r="G31" s="138"/>
+      <c r="H31" s="129"/>
+      <c r="J31" s="125"/>
+      <c r="K31" s="125"/>
+      <c r="L31" s="125"/>
+      <c r="M31" s="125"/>
+      <c r="N31" s="125"/>
+    </row>
+    <row r="32" spans="1:14" s="37" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="99"/>
       <c r="B32" s="92"/>
       <c r="C32" s="41" t="s">
-        <v>157</v>
+        <v>42</v>
       </c>
       <c r="D32" s="94" t="s">
         <v>99</v>
       </c>
       <c r="E32" s="94" t="s">
-        <v>43</v>
+        <v>156</v>
       </c>
       <c r="F32" s="41"/>
       <c r="G32" s="137"/>
@@ -34425,20 +34442,20 @@
       <c r="N32" s="103"/>
     </row>
     <row r="33" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="100"/>
-      <c r="B33" s="93"/>
-      <c r="C33" s="44" t="s">
-        <v>160</v>
+      <c r="A33" s="99"/>
+      <c r="B33" s="92"/>
+      <c r="C33" s="41" t="s">
+        <v>159</v>
       </c>
-      <c r="D33" s="95" t="s">
+      <c r="D33" s="94" t="s">
         <v>99</v>
       </c>
-      <c r="E33" s="95" t="s">
-        <v>161</v>
+      <c r="E33" s="94" t="s">
+        <v>158</v>
       </c>
-      <c r="F33" s="44"/>
-      <c r="G33" s="139"/>
-      <c r="H33" s="45" t="s">
+      <c r="F33" s="41"/>
+      <c r="G33" s="137"/>
+      <c r="H33" s="42" t="s">
         <v>46</v>
       </c>
       <c r="J33" s="103"/>
@@ -34447,40 +34464,44 @@
       <c r="M33" s="103"/>
       <c r="N33" s="103"/>
     </row>
-    <row r="34" spans="1:14" s="124" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="123"/>
-      <c r="B34" s="135" t="s">
-        <v>44</v>
+    <row r="34" spans="1:14" s="37" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="100"/>
+      <c r="B34" s="92"/>
+      <c r="C34" s="41" t="s">
+        <v>157</v>
       </c>
-      <c r="C34" s="136"/>
-      <c r="D34" s="126"/>
-      <c r="E34" s="127"/>
-      <c r="F34" s="127"/>
-      <c r="G34" s="138"/>
-      <c r="H34" s="129" t="s">
+      <c r="D34" s="94" t="s">
+        <v>99</v>
+      </c>
+      <c r="E34" s="94" t="s">
+        <v>43</v>
+      </c>
+      <c r="F34" s="41"/>
+      <c r="G34" s="137"/>
+      <c r="H34" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="J34" s="125"/>
-      <c r="K34" s="125"/>
-      <c r="L34" s="125"/>
-      <c r="M34" s="125"/>
-      <c r="N34" s="125"/>
-    </row>
-    <row r="35" spans="1:14" s="37" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A35" s="99"/>
-      <c r="B35" s="92"/>
-      <c r="C35" s="41" t="s">
-        <v>166</v>
+      <c r="J34" s="103"/>
+      <c r="K34" s="103"/>
+      <c r="L34" s="103"/>
+      <c r="M34" s="103"/>
+      <c r="N34" s="103"/>
+    </row>
+    <row r="35" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="100"/>
+      <c r="B35" s="93"/>
+      <c r="C35" s="44" t="s">
+        <v>160</v>
       </c>
-      <c r="D35" s="94" t="s">
-        <v>117</v>
+      <c r="D35" s="95" t="s">
+        <v>99</v>
       </c>
-      <c r="E35" s="94" t="s">
-        <v>179</v>
+      <c r="E35" s="95" t="s">
+        <v>161</v>
       </c>
-      <c r="F35" s="41"/>
-      <c r="G35" s="137"/>
-      <c r="H35" s="42" t="s">
+      <c r="F35" s="44"/>
+      <c r="G35" s="139"/>
+      <c r="H35" s="45" t="s">
         <v>46</v>
       </c>
       <c r="J35" s="103"/>
@@ -34489,40 +34510,36 @@
       <c r="M35" s="103"/>
       <c r="N35" s="103"/>
     </row>
-    <row r="36" spans="1:14" s="37" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="99"/>
-      <c r="B36" s="92"/>
-      <c r="C36" s="41" t="s">
-        <v>48</v>
+    <row r="36" spans="1:14" s="124" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="123"/>
+      <c r="B36" s="135" t="s">
+        <v>44</v>
       </c>
-      <c r="D36" s="94" t="s">
-        <v>117</v>
-      </c>
-      <c r="E36" s="94" t="s">
-        <v>173</v>
-      </c>
-      <c r="F36" s="41"/>
-      <c r="G36" s="137"/>
-      <c r="H36" s="42" t="s">
+      <c r="C36" s="136"/>
+      <c r="D36" s="126"/>
+      <c r="E36" s="127"/>
+      <c r="F36" s="127"/>
+      <c r="G36" s="138"/>
+      <c r="H36" s="129" t="s">
         <v>46</v>
       </c>
-      <c r="J36" s="103"/>
-      <c r="K36" s="103"/>
-      <c r="L36" s="103"/>
-      <c r="M36" s="103"/>
-      <c r="N36" s="103"/>
-    </row>
-    <row r="37" spans="1:14" s="37" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="J36" s="125"/>
+      <c r="K36" s="125"/>
+      <c r="L36" s="125"/>
+      <c r="M36" s="125"/>
+      <c r="N36" s="125"/>
+    </row>
+    <row r="37" spans="1:14" s="37" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A37" s="99"/>
       <c r="B37" s="92"/>
       <c r="C37" s="41" t="s">
-        <v>49</v>
+        <v>166</v>
       </c>
       <c r="D37" s="94" t="s">
         <v>117</v>
       </c>
       <c r="E37" s="94" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="F37" s="41"/>
       <c r="G37" s="137"/>
@@ -34535,34 +34552,40 @@
       <c r="M37" s="103"/>
       <c r="N37" s="103"/>
     </row>
-    <row r="38" spans="1:14" s="124" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="123"/>
-      <c r="B38" s="135" t="s">
-        <v>139</v>
+    <row r="38" spans="1:14" s="37" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="99"/>
+      <c r="B38" s="92"/>
+      <c r="C38" s="41" t="s">
+        <v>48</v>
       </c>
-      <c r="C38" s="136"/>
-      <c r="D38" s="126"/>
-      <c r="E38" s="127"/>
-      <c r="F38" s="127"/>
-      <c r="G38" s="138"/>
-      <c r="H38" s="129"/>
-      <c r="J38" s="125"/>
-      <c r="K38" s="125"/>
-      <c r="L38" s="125"/>
-      <c r="M38" s="125"/>
-      <c r="N38" s="125"/>
-    </row>
-    <row r="39" spans="1:14" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="D38" s="94" t="s">
+        <v>117</v>
+      </c>
+      <c r="E38" s="94" t="s">
+        <v>173</v>
+      </c>
+      <c r="F38" s="41"/>
+      <c r="G38" s="137"/>
+      <c r="H38" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="J38" s="103"/>
+      <c r="K38" s="103"/>
+      <c r="L38" s="103"/>
+      <c r="M38" s="103"/>
+      <c r="N38" s="103"/>
+    </row>
+    <row r="39" spans="1:14" s="37" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A39" s="99"/>
       <c r="B39" s="92"/>
       <c r="C39" s="41" t="s">
-        <v>138</v>
+        <v>49</v>
       </c>
       <c r="D39" s="94" t="s">
         <v>117</v>
       </c>
       <c r="E39" s="94" t="s">
-        <v>141</v>
+        <v>168</v>
       </c>
       <c r="F39" s="41"/>
       <c r="G39" s="137"/>
@@ -34575,57 +34598,57 @@
       <c r="M39" s="103"/>
       <c r="N39" s="103"/>
     </row>
-    <row r="40" spans="1:14" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="99"/>
-      <c r="B40" s="92"/>
-      <c r="C40" s="41" t="s">
-        <v>171</v>
+    <row r="40" spans="1:14" s="124" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="123"/>
+      <c r="B40" s="135" t="s">
+        <v>139</v>
       </c>
-      <c r="D40" s="94" t="s">
+      <c r="C40" s="136"/>
+      <c r="D40" s="126"/>
+      <c r="E40" s="127"/>
+      <c r="F40" s="127"/>
+      <c r="G40" s="138"/>
+      <c r="H40" s="129"/>
+      <c r="J40" s="125"/>
+      <c r="K40" s="125"/>
+      <c r="L40" s="125"/>
+      <c r="M40" s="125"/>
+      <c r="N40" s="125"/>
+    </row>
+    <row r="41" spans="1:14" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="99"/>
+      <c r="B41" s="92"/>
+      <c r="C41" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="D41" s="94" t="s">
         <v>117</v>
       </c>
-      <c r="E40" s="94" t="s">
-        <v>140</v>
+      <c r="E41" s="94" t="s">
+        <v>141</v>
       </c>
-      <c r="F40" s="41"/>
-      <c r="G40" s="137"/>
-      <c r="H40" s="42" t="s">
+      <c r="F41" s="41"/>
+      <c r="G41" s="137"/>
+      <c r="H41" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="J40" s="103"/>
-      <c r="K40" s="103"/>
-      <c r="L40" s="103"/>
-      <c r="M40" s="103"/>
-      <c r="N40" s="103"/>
-    </row>
-    <row r="41" spans="1:14" s="124" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="123"/>
-      <c r="B41" s="135" t="s">
-        <v>165</v>
-      </c>
-      <c r="C41" s="136"/>
-      <c r="D41" s="126"/>
-      <c r="E41" s="127"/>
-      <c r="F41" s="127"/>
-      <c r="G41" s="138"/>
-      <c r="H41" s="129"/>
-      <c r="J41" s="125"/>
-      <c r="K41" s="125"/>
-      <c r="L41" s="125"/>
-      <c r="M41" s="125"/>
-      <c r="N41" s="125"/>
-    </row>
-    <row r="42" spans="1:14" s="37" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="J41" s="103"/>
+      <c r="K41" s="103"/>
+      <c r="L41" s="103"/>
+      <c r="M41" s="103"/>
+      <c r="N41" s="103"/>
+    </row>
+    <row r="42" spans="1:14" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="99"/>
       <c r="B42" s="92"/>
       <c r="C42" s="41" t="s">
-        <v>146</v>
+        <v>171</v>
       </c>
       <c r="D42" s="94" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="E42" s="94" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F42" s="41"/>
       <c r="G42" s="137"/>
@@ -34638,40 +34661,34 @@
       <c r="M42" s="103"/>
       <c r="N42" s="103"/>
     </row>
-    <row r="43" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="99"/>
-      <c r="B43" s="92"/>
-      <c r="C43" s="41" t="s">
-        <v>34</v>
+    <row r="43" spans="1:14" s="124" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="123"/>
+      <c r="B43" s="135" t="s">
+        <v>165</v>
       </c>
-      <c r="D43" s="94" t="s">
-        <v>99</v>
-      </c>
-      <c r="E43" s="94" t="s">
-        <v>153</v>
-      </c>
-      <c r="F43" s="41"/>
-      <c r="G43" s="137"/>
-      <c r="H43" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="J43" s="103"/>
-      <c r="K43" s="103"/>
-      <c r="L43" s="103"/>
-      <c r="M43" s="103"/>
-      <c r="N43" s="103"/>
-    </row>
-    <row r="44" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C43" s="136"/>
+      <c r="D43" s="126"/>
+      <c r="E43" s="127"/>
+      <c r="F43" s="127"/>
+      <c r="G43" s="138"/>
+      <c r="H43" s="129"/>
+      <c r="J43" s="125"/>
+      <c r="K43" s="125"/>
+      <c r="L43" s="125"/>
+      <c r="M43" s="125"/>
+      <c r="N43" s="125"/>
+    </row>
+    <row r="44" spans="1:14" s="37" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A44" s="99"/>
       <c r="B44" s="92"/>
       <c r="C44" s="41" t="s">
-        <v>35</v>
+        <v>146</v>
       </c>
       <c r="D44" s="94" t="s">
         <v>99</v>
       </c>
       <c r="E44" s="94" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="F44" s="41"/>
       <c r="G44" s="137"/>
@@ -34688,13 +34705,13 @@
       <c r="A45" s="99"/>
       <c r="B45" s="92"/>
       <c r="C45" s="41" t="s">
-        <v>155</v>
+        <v>34</v>
       </c>
       <c r="D45" s="94" t="s">
         <v>99</v>
       </c>
       <c r="E45" s="94" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F45" s="41"/>
       <c r="G45" s="137"/>
@@ -34707,17 +34724,17 @@
       <c r="M45" s="103"/>
       <c r="N45" s="103"/>
     </row>
-    <row r="46" spans="1:14" s="37" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="100"/>
+    <row r="46" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="99"/>
       <c r="B46" s="92"/>
       <c r="C46" s="41" t="s">
-        <v>147</v>
+        <v>35</v>
       </c>
       <c r="D46" s="94" t="s">
         <v>99</v>
       </c>
       <c r="E46" s="94" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="F46" s="41"/>
       <c r="G46" s="137"/>
@@ -34731,16 +34748,16 @@
       <c r="N46" s="103"/>
     </row>
     <row r="47" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="100"/>
+      <c r="A47" s="99"/>
       <c r="B47" s="92"/>
       <c r="C47" s="41" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="D47" s="94" t="s">
         <v>99</v>
       </c>
       <c r="E47" s="94" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="F47" s="41"/>
       <c r="G47" s="137"/>
@@ -34753,15 +34770,17 @@
       <c r="M47" s="103"/>
       <c r="N47" s="103"/>
     </row>
-    <row r="48" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" s="37" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A48" s="100"/>
       <c r="B48" s="92"/>
       <c r="C48" s="41" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
-      <c r="D48" s="94"/>
+      <c r="D48" s="94" t="s">
+        <v>99</v>
+      </c>
       <c r="E48" s="94" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="F48" s="41"/>
       <c r="G48" s="137"/>
@@ -34774,17 +34793,17 @@
       <c r="M48" s="103"/>
       <c r="N48" s="103"/>
     </row>
-    <row r="49" spans="1:14" s="37" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="100"/>
       <c r="B49" s="92"/>
       <c r="C49" s="41" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D49" s="94" t="s">
         <v>99</v>
       </c>
       <c r="E49" s="94" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="F49" s="41"/>
       <c r="G49" s="137"/>
@@ -34800,17 +34819,15 @@
     <row r="50" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="100"/>
       <c r="B50" s="92"/>
-      <c r="C50" s="141" t="s">
-        <v>49</v>
+      <c r="C50" s="41" t="s">
+        <v>163</v>
       </c>
-      <c r="D50" s="94" t="s">
-        <v>99</v>
+      <c r="D50" s="94"/>
+      <c r="E50" s="94" t="s">
+        <v>164</v>
       </c>
-      <c r="E50" s="142" t="s">
-        <v>181</v>
-      </c>
-      <c r="F50" s="141"/>
-      <c r="G50" s="143"/>
+      <c r="F50" s="41"/>
+      <c r="G50" s="137"/>
       <c r="H50" s="42" t="s">
         <v>46</v>
       </c>
@@ -34820,18 +34837,20 @@
       <c r="M50" s="103"/>
       <c r="N50" s="103"/>
     </row>
-    <row r="51" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" s="37" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A51" s="100"/>
       <c r="B51" s="92"/>
-      <c r="C51" s="141" t="s">
-        <v>178</v>
+      <c r="C51" s="41" t="s">
+        <v>169</v>
       </c>
       <c r="D51" s="94" t="s">
         <v>99</v>
       </c>
-      <c r="E51" s="142"/>
-      <c r="F51" s="141"/>
-      <c r="G51" s="143"/>
+      <c r="E51" s="94" t="s">
+        <v>180</v>
+      </c>
+      <c r="F51" s="41"/>
+      <c r="G51" s="137"/>
       <c r="H51" s="42" t="s">
         <v>46</v>
       </c>
@@ -34843,17 +34862,19 @@
     </row>
     <row r="52" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="100"/>
-      <c r="B52" s="93"/>
-      <c r="C52" s="44" t="s">
-        <v>172</v>
+      <c r="B52" s="92"/>
+      <c r="C52" s="141" t="s">
+        <v>49</v>
       </c>
-      <c r="D52" s="95" t="s">
+      <c r="D52" s="94" t="s">
         <v>99</v>
       </c>
-      <c r="E52" s="95"/>
-      <c r="F52" s="44"/>
-      <c r="G52" s="139"/>
-      <c r="H52" s="45" t="s">
+      <c r="E52" s="142" t="s">
+        <v>181</v>
+      </c>
+      <c r="F52" s="141"/>
+      <c r="G52" s="143"/>
+      <c r="H52" s="42" t="s">
         <v>46</v>
       </c>
       <c r="J52" s="103"/>
@@ -34864,13 +34885,19 @@
     </row>
     <row r="53" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="100"/>
-      <c r="B53" s="117"/>
-      <c r="C53" s="36"/>
-      <c r="D53" s="106"/>
-      <c r="E53" s="36"/>
-      <c r="F53" s="36"/>
-      <c r="G53" s="43"/>
-      <c r="H53" s="43"/>
+      <c r="B53" s="92"/>
+      <c r="C53" s="141" t="s">
+        <v>178</v>
+      </c>
+      <c r="D53" s="94" t="s">
+        <v>99</v>
+      </c>
+      <c r="E53" s="142"/>
+      <c r="F53" s="141"/>
+      <c r="G53" s="143"/>
+      <c r="H53" s="42" t="s">
+        <v>46</v>
+      </c>
       <c r="J53" s="103"/>
       <c r="K53" s="103"/>
       <c r="L53" s="103"/>
@@ -34879,17 +34906,24 @@
     </row>
     <row r="54" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="100"/>
-      <c r="B54" s="117"/>
-      <c r="C54" s="36"/>
-      <c r="D54" s="106"/>
-      <c r="E54" s="36"/>
-      <c r="F54" s="36"/>
-      <c r="G54" s="43"/>
-      <c r="I54" s="103"/>
+      <c r="B54" s="93"/>
+      <c r="C54" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="D54" s="95" t="s">
+        <v>99</v>
+      </c>
+      <c r="E54" s="95"/>
+      <c r="F54" s="44"/>
+      <c r="G54" s="139"/>
+      <c r="H54" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="J54" s="103"/>
       <c r="K54" s="103"/>
       <c r="L54" s="103"/>
       <c r="M54" s="103"/>
+      <c r="N54" s="103"/>
     </row>
     <row r="55" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="100"/>
@@ -34899,11 +34933,12 @@
       <c r="E55" s="36"/>
       <c r="F55" s="36"/>
       <c r="G55" s="43"/>
-      <c r="I55" s="103"/>
+      <c r="H55" s="43"/>
       <c r="J55" s="103"/>
       <c r="K55" s="103"/>
       <c r="L55" s="103"/>
       <c r="M55" s="103"/>
+      <c r="N55" s="103"/>
     </row>
     <row r="56" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="100"/>
@@ -34947,11 +34982,9 @@
       <c r="L58" s="103"/>
       <c r="M58" s="103"/>
     </row>
-    <row r="59" spans="1:14" s="37" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="100"/>
-      <c r="B59" s="118" t="s">
-        <v>51</v>
-      </c>
+      <c r="B59" s="117"/>
       <c r="C59" s="36"/>
       <c r="D59" s="106"/>
       <c r="E59" s="36"/>
@@ -34965,11 +34998,11 @@
     </row>
     <row r="60" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="100"/>
-      <c r="B60" s="20"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="101"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
+      <c r="B60" s="117"/>
+      <c r="C60" s="36"/>
+      <c r="D60" s="106"/>
+      <c r="E60" s="36"/>
+      <c r="F60" s="36"/>
       <c r="G60" s="43"/>
       <c r="I60" s="103"/>
       <c r="J60" s="103"/>
@@ -34977,21 +35010,15 @@
       <c r="L60" s="103"/>
       <c r="M60" s="103"/>
     </row>
-    <row r="61" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" s="37" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A61" s="100"/>
-      <c r="B61" s="119" t="s">
-        <v>33</v>
+      <c r="B61" s="118" t="s">
+        <v>51</v>
       </c>
-      <c r="C61" s="52" t="s">
-        <v>52</v>
-      </c>
-      <c r="D61" s="107"/>
-      <c r="E61" s="52" t="s">
-        <v>53</v>
-      </c>
-      <c r="F61" s="53" t="s">
-        <v>54</v>
-      </c>
+      <c r="C61" s="36"/>
+      <c r="D61" s="106"/>
+      <c r="E61" s="36"/>
+      <c r="F61" s="36"/>
       <c r="G61" s="43"/>
       <c r="I61" s="103"/>
       <c r="J61" s="103"/>
@@ -35001,19 +35028,11 @@
     </row>
     <row r="62" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="100"/>
-      <c r="B62" s="91" t="s">
-        <v>55</v>
-      </c>
-      <c r="C62" s="46" t="s">
-        <v>56</v>
-      </c>
-      <c r="D62" s="108"/>
-      <c r="E62" s="46" t="s">
-        <v>57</v>
-      </c>
-      <c r="F62" s="47" t="s">
-        <v>58</v>
-      </c>
+      <c r="B62" s="20"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="101"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
       <c r="G62" s="43"/>
       <c r="I62" s="103"/>
       <c r="J62" s="103"/>
@@ -35023,13 +35042,19 @@
     </row>
     <row r="63" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="100"/>
-      <c r="B63" s="92"/>
-      <c r="C63" s="48" t="s">
-        <v>59</v>
+      <c r="B63" s="119" t="s">
+        <v>33</v>
       </c>
-      <c r="D63" s="109"/>
-      <c r="E63" s="48"/>
-      <c r="F63" s="49"/>
+      <c r="C63" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="D63" s="107"/>
+      <c r="E63" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="F63" s="53" t="s">
+        <v>54</v>
+      </c>
       <c r="G63" s="43"/>
       <c r="I63" s="103"/>
       <c r="J63" s="103"/>
@@ -35039,14 +35064,18 @@
     </row>
     <row r="64" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="100"/>
-      <c r="B64" s="92"/>
-      <c r="C64" s="48" t="s">
-        <v>60</v>
+      <c r="B64" s="91" t="s">
+        <v>55</v>
       </c>
-      <c r="D64" s="109"/>
-      <c r="E64" s="48"/>
-      <c r="F64" s="49" t="s">
-        <v>61</v>
+      <c r="C64" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="D64" s="108"/>
+      <c r="E64" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="F64" s="47" t="s">
+        <v>58</v>
       </c>
       <c r="G64" s="43"/>
       <c r="I64" s="103"/>
@@ -35059,13 +35088,11 @@
       <c r="A65" s="100"/>
       <c r="B65" s="92"/>
       <c r="C65" s="48" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D65" s="109"/>
       <c r="E65" s="48"/>
-      <c r="F65" s="49" t="s">
-        <v>63</v>
-      </c>
+      <c r="F65" s="49"/>
       <c r="G65" s="43"/>
       <c r="I65" s="103"/>
       <c r="J65" s="103"/>
@@ -35075,13 +35102,15 @@
     </row>
     <row r="66" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="100"/>
-      <c r="B66" s="93"/>
-      <c r="C66" s="54" t="s">
-        <v>64</v>
+      <c r="B66" s="92"/>
+      <c r="C66" s="48" t="s">
+        <v>60</v>
       </c>
-      <c r="D66" s="110"/>
-      <c r="E66" s="54"/>
-      <c r="F66" s="55"/>
+      <c r="D66" s="109"/>
+      <c r="E66" s="48"/>
+      <c r="F66" s="49" t="s">
+        <v>61</v>
+      </c>
       <c r="G66" s="43"/>
       <c r="I66" s="103"/>
       <c r="J66" s="103"/>
@@ -35089,20 +35118,16 @@
       <c r="L66" s="103"/>
       <c r="M66" s="103"/>
     </row>
-    <row r="67" spans="1:13" s="37" customFormat="1" ht="42" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="100"/>
-      <c r="B67" s="89" t="s">
-        <v>65</v>
+      <c r="B67" s="92"/>
+      <c r="C67" s="48" t="s">
+        <v>62</v>
       </c>
-      <c r="C67" s="61" t="s">
-        <v>66</v>
-      </c>
-      <c r="D67" s="111"/>
-      <c r="E67" s="61" t="s">
-        <v>67</v>
-      </c>
-      <c r="F67" s="68" t="s">
-        <v>85</v>
+      <c r="D67" s="109"/>
+      <c r="E67" s="48"/>
+      <c r="F67" s="49" t="s">
+        <v>63</v>
       </c>
       <c r="G67" s="43"/>
       <c r="I67" s="103"/>
@@ -35113,17 +35138,13 @@
     </row>
     <row r="68" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="100"/>
-      <c r="B68" s="90"/>
-      <c r="C68" s="62" t="s">
-        <v>68</v>
+      <c r="B68" s="93"/>
+      <c r="C68" s="54" t="s">
+        <v>64</v>
       </c>
-      <c r="D68" s="112"/>
-      <c r="E68" s="62" t="s">
-        <v>68</v>
-      </c>
-      <c r="F68" s="63" t="s">
-        <v>69</v>
-      </c>
+      <c r="D68" s="110"/>
+      <c r="E68" s="54"/>
+      <c r="F68" s="55"/>
       <c r="G68" s="43"/>
       <c r="I68" s="103"/>
       <c r="J68" s="103"/>
@@ -35131,20 +35152,20 @@
       <c r="L68" s="103"/>
       <c r="M68" s="103"/>
     </row>
-    <row r="69" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" s="37" customFormat="1" ht="42" x14ac:dyDescent="0.25">
       <c r="A69" s="100"/>
-      <c r="B69" s="91" t="s">
-        <v>70</v>
+      <c r="B69" s="89" t="s">
+        <v>65</v>
       </c>
-      <c r="C69" s="58" t="s">
-        <v>71</v>
+      <c r="C69" s="61" t="s">
+        <v>66</v>
       </c>
-      <c r="D69" s="113"/>
-      <c r="E69" s="58" t="s">
-        <v>72</v>
+      <c r="D69" s="111"/>
+      <c r="E69" s="61" t="s">
+        <v>67</v>
       </c>
-      <c r="F69" s="59" t="s">
-        <v>73</v>
+      <c r="F69" s="68" t="s">
+        <v>85</v>
       </c>
       <c r="G69" s="43"/>
       <c r="I69" s="103"/>
@@ -35155,14 +35176,16 @@
     </row>
     <row r="70" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="100"/>
-      <c r="B70" s="93"/>
-      <c r="C70" s="54"/>
-      <c r="D70" s="110"/>
-      <c r="E70" s="56" t="s">
-        <v>74</v>
+      <c r="B70" s="90"/>
+      <c r="C70" s="62" t="s">
+        <v>68</v>
       </c>
-      <c r="F70" s="57" t="s">
-        <v>75</v>
+      <c r="D70" s="112"/>
+      <c r="E70" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="F70" s="63" t="s">
+        <v>69</v>
       </c>
       <c r="G70" s="43"/>
       <c r="I70" s="103"/>
@@ -35173,18 +35196,18 @@
     </row>
     <row r="71" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="100"/>
-      <c r="B71" s="67" t="s">
-        <v>76</v>
+      <c r="B71" s="91" t="s">
+        <v>70</v>
       </c>
-      <c r="C71" s="64" t="s">
-        <v>77</v>
+      <c r="C71" s="58" t="s">
+        <v>71</v>
       </c>
-      <c r="D71" s="114"/>
-      <c r="E71" s="65">
-        <v>2013</v>
+      <c r="D71" s="113"/>
+      <c r="E71" s="58" t="s">
+        <v>72</v>
       </c>
-      <c r="F71" s="66" t="s">
-        <v>78</v>
+      <c r="F71" s="59" t="s">
+        <v>73</v>
       </c>
       <c r="G71" s="43"/>
       <c r="I71" s="103"/>
@@ -35195,18 +35218,14 @@
     </row>
     <row r="72" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="100"/>
-      <c r="B72" s="91" t="s">
-        <v>79</v>
+      <c r="B72" s="93"/>
+      <c r="C72" s="54"/>
+      <c r="D72" s="110"/>
+      <c r="E72" s="56" t="s">
+        <v>74</v>
       </c>
-      <c r="C72" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="D72" s="108"/>
-      <c r="E72" s="46" t="s">
-        <v>81</v>
-      </c>
-      <c r="F72" s="47" t="s">
-        <v>82</v>
+      <c r="F72" s="57" t="s">
+        <v>75</v>
       </c>
       <c r="G72" s="43"/>
       <c r="I72" s="103"/>
@@ -35215,18 +35234,20 @@
       <c r="L72" s="103"/>
       <c r="M72" s="103"/>
     </row>
-    <row r="73" spans="1:13" s="37" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="100"/>
-      <c r="B73" s="92"/>
-      <c r="C73" s="48" t="s">
-        <v>83</v>
+      <c r="B73" s="67" t="s">
+        <v>76</v>
       </c>
-      <c r="D73" s="109"/>
-      <c r="E73" s="48" t="s">
-        <v>83</v>
+      <c r="C73" s="64" t="s">
+        <v>77</v>
       </c>
-      <c r="F73" s="50" t="s">
-        <v>86</v>
+      <c r="D73" s="114"/>
+      <c r="E73" s="65">
+        <v>2013</v>
+      </c>
+      <c r="F73" s="66" t="s">
+        <v>78</v>
       </c>
       <c r="G73" s="43"/>
       <c r="I73" s="103"/>
@@ -35237,13 +35258,19 @@
     </row>
     <row r="74" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="100"/>
-      <c r="B74" s="92"/>
-      <c r="C74" s="48" t="s">
-        <v>84</v>
+      <c r="B74" s="91" t="s">
+        <v>79</v>
       </c>
-      <c r="D74" s="109"/>
-      <c r="E74" s="48"/>
-      <c r="F74" s="49"/>
+      <c r="C74" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="D74" s="108"/>
+      <c r="E74" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="F74" s="47" t="s">
+        <v>82</v>
+      </c>
       <c r="G74" s="43"/>
       <c r="I74" s="103"/>
       <c r="J74" s="103"/>
@@ -35251,16 +35278,18 @@
       <c r="L74" s="103"/>
       <c r="M74" s="103"/>
     </row>
-    <row r="75" spans="1:13" s="37" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" s="37" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A75" s="100"/>
-      <c r="B75" s="93"/>
-      <c r="C75" s="60" t="s">
-        <v>68</v>
+      <c r="B75" s="92"/>
+      <c r="C75" s="48" t="s">
+        <v>83</v>
       </c>
-      <c r="D75" s="115"/>
-      <c r="E75" s="60"/>
-      <c r="F75" s="51" t="s">
-        <v>87</v>
+      <c r="D75" s="109"/>
+      <c r="E75" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="F75" s="50" t="s">
+        <v>86</v>
       </c>
       <c r="G75" s="43"/>
       <c r="I75" s="103"/>
@@ -35271,11 +35300,13 @@
     </row>
     <row r="76" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="100"/>
-      <c r="B76" s="117"/>
-      <c r="C76" s="36"/>
-      <c r="D76" s="106"/>
-      <c r="E76" s="36"/>
-      <c r="F76" s="36"/>
+      <c r="B76" s="92"/>
+      <c r="C76" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="D76" s="109"/>
+      <c r="E76" s="48"/>
+      <c r="F76" s="49"/>
       <c r="G76" s="43"/>
       <c r="I76" s="103"/>
       <c r="J76" s="103"/>
@@ -35283,13 +35314,17 @@
       <c r="L76" s="103"/>
       <c r="M76" s="103"/>
     </row>
-    <row r="77" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" s="37" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A77" s="100"/>
-      <c r="B77" s="117"/>
-      <c r="C77" s="36"/>
-      <c r="D77" s="106"/>
-      <c r="E77" s="36"/>
-      <c r="F77" s="36"/>
+      <c r="B77" s="93"/>
+      <c r="C77" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="D77" s="115"/>
+      <c r="E77" s="60"/>
+      <c r="F77" s="51" t="s">
+        <v>87</v>
+      </c>
       <c r="G77" s="43"/>
       <c r="I77" s="103"/>
       <c r="J77" s="103"/>
@@ -36249,33 +36284,33 @@
       <c r="L145" s="103"/>
       <c r="M145" s="103"/>
     </row>
-    <row r="146" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="97"/>
+    <row r="146" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="100"/>
       <c r="B146" s="117"/>
-      <c r="C146" s="1"/>
-      <c r="D146" s="101"/>
-      <c r="E146" s="1"/>
-      <c r="F146" s="1"/>
-      <c r="G146" s="39"/>
-      <c r="I146" s="102"/>
-      <c r="J146" s="102"/>
-      <c r="K146" s="102"/>
-      <c r="L146" s="102"/>
-      <c r="M146" s="102"/>
-    </row>
-    <row r="147" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="97"/>
+      <c r="C146" s="36"/>
+      <c r="D146" s="106"/>
+      <c r="E146" s="36"/>
+      <c r="F146" s="36"/>
+      <c r="G146" s="43"/>
+      <c r="I146" s="103"/>
+      <c r="J146" s="103"/>
+      <c r="K146" s="103"/>
+      <c r="L146" s="103"/>
+      <c r="M146" s="103"/>
+    </row>
+    <row r="147" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="100"/>
       <c r="B147" s="117"/>
-      <c r="C147" s="1"/>
-      <c r="D147" s="101"/>
-      <c r="E147" s="1"/>
-      <c r="F147" s="1"/>
-      <c r="G147" s="39"/>
-      <c r="I147" s="102"/>
-      <c r="J147" s="102"/>
-      <c r="K147" s="102"/>
-      <c r="L147" s="102"/>
-      <c r="M147" s="102"/>
+      <c r="C147" s="36"/>
+      <c r="D147" s="106"/>
+      <c r="E147" s="36"/>
+      <c r="F147" s="36"/>
+      <c r="G147" s="43"/>
+      <c r="I147" s="103"/>
+      <c r="J147" s="103"/>
+      <c r="K147" s="103"/>
+      <c r="L147" s="103"/>
+      <c r="M147" s="103"/>
     </row>
     <row r="148" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="97"/>
@@ -37929,15 +37964,33 @@
       <c r="L265" s="102"/>
       <c r="M265" s="102"/>
     </row>
-    <row r="266" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H266" s="1"/>
-      <c r="I266" s="101"/>
-      <c r="N266" s="1"/>
-    </row>
-    <row r="267" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H267" s="1"/>
-      <c r="I267" s="101"/>
-      <c r="N267" s="1"/>
+    <row r="266" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A266" s="97"/>
+      <c r="B266" s="117"/>
+      <c r="C266" s="1"/>
+      <c r="D266" s="101"/>
+      <c r="E266" s="1"/>
+      <c r="F266" s="1"/>
+      <c r="G266" s="39"/>
+      <c r="I266" s="102"/>
+      <c r="J266" s="102"/>
+      <c r="K266" s="102"/>
+      <c r="L266" s="102"/>
+      <c r="M266" s="102"/>
+    </row>
+    <row r="267" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A267" s="97"/>
+      <c r="B267" s="117"/>
+      <c r="C267" s="1"/>
+      <c r="D267" s="101"/>
+      <c r="E267" s="1"/>
+      <c r="F267" s="1"/>
+      <c r="G267" s="39"/>
+      <c r="I267" s="102"/>
+      <c r="J267" s="102"/>
+      <c r="K267" s="102"/>
+      <c r="L267" s="102"/>
+      <c r="M267" s="102"/>
     </row>
     <row r="268" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H268" s="1"/>
@@ -42209,8 +42262,18 @@
       <c r="I1121" s="101"/>
       <c r="N1121" s="1"/>
     </row>
+    <row r="1122" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H1122" s="1"/>
+      <c r="I1122" s="101"/>
+      <c r="N1122" s="1"/>
+    </row>
+    <row r="1123" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H1123" s="1"/>
+      <c r="I1123" s="101"/>
+      <c r="N1123" s="1"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="H11:H14 H16:H20 H39:H40 H42:H46 H9 H22:H28 H30:H33">
+  <conditionalFormatting sqref="H11:H14 H41:H42 H44:H48 H9 H24:H30 H32:H35 H16:H22">
     <cfRule type="cellIs" dxfId="13" priority="45" operator="equal">
       <formula>$A$11</formula>
     </cfRule>
@@ -42218,7 +42281,7 @@
       <formula>$A$7</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H48:H51">
+  <conditionalFormatting sqref="H50:H53">
     <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
       <formula>$A$11</formula>
     </cfRule>
@@ -42226,7 +42289,7 @@
       <formula>$A$7</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H47">
+  <conditionalFormatting sqref="H49">
     <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
       <formula>$A$11</formula>
     </cfRule>
@@ -42234,7 +42297,7 @@
       <formula>$A$7</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
+  <conditionalFormatting sqref="H37">
     <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
       <formula>$A$11</formula>
     </cfRule>
@@ -42242,7 +42305,7 @@
       <formula>$A$7</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H36:H37">
+  <conditionalFormatting sqref="H38:H39">
     <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
       <formula>$A$11</formula>
     </cfRule>
@@ -42250,7 +42313,7 @@
       <formula>$A$7</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H33">
+  <conditionalFormatting sqref="H35">
     <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>$A$11</formula>
     </cfRule>
@@ -42258,7 +42321,7 @@
       <formula>$A$7</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H52">
+  <conditionalFormatting sqref="H54">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>$A$11</formula>
     </cfRule>
@@ -42267,10 +42330,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H9 H11:H52" xr:uid="{38080977-4269-4EAA-AF58-F25EAE9C07B6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H9 H11:H54" xr:uid="{38080977-4269-4EAA-AF58-F25EAE9C07B6}">
       <formula1>$L$7:$L$8</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:D9 D11:D52" xr:uid="{3B8CE9F0-680B-4E0A-B694-A1F2EA07B84E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:D9 D11:D54" xr:uid="{3B8CE9F0-680B-4E0A-B694-A1F2EA07B84E}">
       <formula1>$J$7:$J$10</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Fachadministrator in Install Anleitung aufgenommen.
</commit_message>
<xml_diff>
--- a/8. Harmonising standards/01_Project organisation/03_Project Documentation/Template Project Documentation 1.1.xlsx
+++ b/8. Harmonising standards/01_Project organisation/03_Project Documentation/Template Project Documentation 1.1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC62AC4E-2C17-4278-82A6-B891D46E1533}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F404D1-ED9C-4733-96FA-330AB8D7F0C7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="4725" tabRatio="837" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="196">
   <si>
     <t>Corporate Design</t>
   </si>
@@ -719,6 +719,12 @@
   </si>
   <si>
     <t>RAM Nutzung des SQL Servers auf ca. 2/3 der Server RAM begrenzen</t>
+  </si>
+  <si>
+    <t>User Domäne\[Fachadministrator] als Admin berechtigen</t>
+  </si>
+  <si>
+    <t>User per Script als Admin berechtigen</t>
   </si>
 </sst>
 </file>
@@ -33758,12 +33764,12 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:N1123"/>
+  <dimension ref="A1:N1124"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H33" sqref="H33"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34376,22 +34382,20 @@
       <c r="M29" s="103"/>
       <c r="N29" s="103"/>
     </row>
-    <row r="30" spans="1:14" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="99"/>
       <c r="B30" s="92"/>
       <c r="C30" s="120" t="s">
-        <v>144</v>
+        <v>194</v>
       </c>
       <c r="D30" s="121" t="s">
         <v>99</v>
       </c>
       <c r="E30" s="121" t="s">
-        <v>176</v>
+        <v>195</v>
       </c>
       <c r="F30" s="120"/>
-      <c r="G30" s="140" t="s">
-        <v>177</v>
-      </c>
+      <c r="G30" s="140"/>
       <c r="H30" s="122" t="s">
         <v>46</v>
       </c>
@@ -34401,57 +34405,59 @@
       <c r="M30" s="103"/>
       <c r="N30" s="103"/>
     </row>
-    <row r="31" spans="1:14" s="124" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="123"/>
-      <c r="B31" s="135" t="s">
+    <row r="31" spans="1:14" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="99"/>
+      <c r="B31" s="92"/>
+      <c r="C31" s="120" t="s">
+        <v>144</v>
+      </c>
+      <c r="D31" s="121" t="s">
+        <v>99</v>
+      </c>
+      <c r="E31" s="121" t="s">
+        <v>176</v>
+      </c>
+      <c r="F31" s="120"/>
+      <c r="G31" s="140" t="s">
+        <v>177</v>
+      </c>
+      <c r="H31" s="122" t="s">
+        <v>46</v>
+      </c>
+      <c r="J31" s="103"/>
+      <c r="K31" s="103"/>
+      <c r="L31" s="103"/>
+      <c r="M31" s="103"/>
+      <c r="N31" s="103"/>
+    </row>
+    <row r="32" spans="1:14" s="124" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="123"/>
+      <c r="B32" s="135" t="s">
         <v>170</v>
       </c>
-      <c r="C31" s="136"/>
-      <c r="D31" s="126"/>
-      <c r="E31" s="127"/>
-      <c r="F31" s="127"/>
-      <c r="G31" s="138"/>
-      <c r="H31" s="129"/>
-      <c r="J31" s="125"/>
-      <c r="K31" s="125"/>
-      <c r="L31" s="125"/>
-      <c r="M31" s="125"/>
-      <c r="N31" s="125"/>
-    </row>
-    <row r="32" spans="1:14" s="37" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="99"/>
-      <c r="B32" s="92"/>
-      <c r="C32" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="D32" s="94" t="s">
-        <v>99</v>
-      </c>
-      <c r="E32" s="94" t="s">
-        <v>156</v>
-      </c>
-      <c r="F32" s="41"/>
-      <c r="G32" s="137"/>
-      <c r="H32" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="J32" s="103"/>
-      <c r="K32" s="103"/>
-      <c r="L32" s="103"/>
-      <c r="M32" s="103"/>
-      <c r="N32" s="103"/>
-    </row>
-    <row r="33" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="136"/>
+      <c r="D32" s="126"/>
+      <c r="E32" s="127"/>
+      <c r="F32" s="127"/>
+      <c r="G32" s="138"/>
+      <c r="H32" s="129"/>
+      <c r="J32" s="125"/>
+      <c r="K32" s="125"/>
+      <c r="L32" s="125"/>
+      <c r="M32" s="125"/>
+      <c r="N32" s="125"/>
+    </row>
+    <row r="33" spans="1:14" s="37" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A33" s="99"/>
       <c r="B33" s="92"/>
       <c r="C33" s="41" t="s">
-        <v>159</v>
+        <v>42</v>
       </c>
       <c r="D33" s="94" t="s">
         <v>99</v>
       </c>
       <c r="E33" s="94" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F33" s="41"/>
       <c r="G33" s="137"/>
@@ -34464,17 +34470,17 @@
       <c r="M33" s="103"/>
       <c r="N33" s="103"/>
     </row>
-    <row r="34" spans="1:14" s="37" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="100"/>
+    <row r="34" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="99"/>
       <c r="B34" s="92"/>
       <c r="C34" s="41" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D34" s="94" t="s">
         <v>99</v>
       </c>
       <c r="E34" s="94" t="s">
-        <v>43</v>
+        <v>158</v>
       </c>
       <c r="F34" s="41"/>
       <c r="G34" s="137"/>
@@ -34487,21 +34493,21 @@
       <c r="M34" s="103"/>
       <c r="N34" s="103"/>
     </row>
-    <row r="35" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" s="37" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A35" s="100"/>
-      <c r="B35" s="93"/>
-      <c r="C35" s="44" t="s">
-        <v>160</v>
+      <c r="B35" s="92"/>
+      <c r="C35" s="41" t="s">
+        <v>157</v>
       </c>
-      <c r="D35" s="95" t="s">
+      <c r="D35" s="94" t="s">
         <v>99</v>
       </c>
-      <c r="E35" s="95" t="s">
-        <v>161</v>
+      <c r="E35" s="94" t="s">
+        <v>43</v>
       </c>
-      <c r="F35" s="44"/>
-      <c r="G35" s="139"/>
-      <c r="H35" s="45" t="s">
+      <c r="F35" s="41"/>
+      <c r="G35" s="137"/>
+      <c r="H35" s="42" t="s">
         <v>46</v>
       </c>
       <c r="J35" s="103"/>
@@ -34510,59 +34516,59 @@
       <c r="M35" s="103"/>
       <c r="N35" s="103"/>
     </row>
-    <row r="36" spans="1:14" s="124" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="123"/>
-      <c r="B36" s="135" t="s">
+    <row r="36" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="100"/>
+      <c r="B36" s="93"/>
+      <c r="C36" s="44" t="s">
+        <v>160</v>
+      </c>
+      <c r="D36" s="95" t="s">
+        <v>99</v>
+      </c>
+      <c r="E36" s="95" t="s">
+        <v>161</v>
+      </c>
+      <c r="F36" s="44"/>
+      <c r="G36" s="139"/>
+      <c r="H36" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="J36" s="103"/>
+      <c r="K36" s="103"/>
+      <c r="L36" s="103"/>
+      <c r="M36" s="103"/>
+      <c r="N36" s="103"/>
+    </row>
+    <row r="37" spans="1:14" s="124" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="123"/>
+      <c r="B37" s="135" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="136"/>
-      <c r="D36" s="126"/>
-      <c r="E36" s="127"/>
-      <c r="F36" s="127"/>
-      <c r="G36" s="138"/>
-      <c r="H36" s="129" t="s">
+      <c r="C37" s="136"/>
+      <c r="D37" s="126"/>
+      <c r="E37" s="127"/>
+      <c r="F37" s="127"/>
+      <c r="G37" s="138"/>
+      <c r="H37" s="129" t="s">
         <v>46</v>
       </c>
-      <c r="J36" s="125"/>
-      <c r="K36" s="125"/>
-      <c r="L36" s="125"/>
-      <c r="M36" s="125"/>
-      <c r="N36" s="125"/>
-    </row>
-    <row r="37" spans="1:14" s="37" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A37" s="99"/>
-      <c r="B37" s="92"/>
-      <c r="C37" s="41" t="s">
-        <v>166</v>
-      </c>
-      <c r="D37" s="94" t="s">
-        <v>117</v>
-      </c>
-      <c r="E37" s="94" t="s">
-        <v>179</v>
-      </c>
-      <c r="F37" s="41"/>
-      <c r="G37" s="137"/>
-      <c r="H37" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="J37" s="103"/>
-      <c r="K37" s="103"/>
-      <c r="L37" s="103"/>
-      <c r="M37" s="103"/>
-      <c r="N37" s="103"/>
-    </row>
-    <row r="38" spans="1:14" s="37" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="J37" s="125"/>
+      <c r="K37" s="125"/>
+      <c r="L37" s="125"/>
+      <c r="M37" s="125"/>
+      <c r="N37" s="125"/>
+    </row>
+    <row r="38" spans="1:14" s="37" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A38" s="99"/>
       <c r="B38" s="92"/>
       <c r="C38" s="41" t="s">
-        <v>48</v>
+        <v>166</v>
       </c>
       <c r="D38" s="94" t="s">
         <v>117</v>
       </c>
       <c r="E38" s="94" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="F38" s="41"/>
       <c r="G38" s="137"/>
@@ -34579,13 +34585,13 @@
       <c r="A39" s="99"/>
       <c r="B39" s="92"/>
       <c r="C39" s="41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D39" s="94" t="s">
         <v>117</v>
       </c>
       <c r="E39" s="94" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="F39" s="41"/>
       <c r="G39" s="137"/>
@@ -34598,57 +34604,57 @@
       <c r="M39" s="103"/>
       <c r="N39" s="103"/>
     </row>
-    <row r="40" spans="1:14" s="124" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="123"/>
-      <c r="B40" s="135" t="s">
+    <row r="40" spans="1:14" s="37" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="99"/>
+      <c r="B40" s="92"/>
+      <c r="C40" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="D40" s="94" t="s">
+        <v>117</v>
+      </c>
+      <c r="E40" s="94" t="s">
+        <v>168</v>
+      </c>
+      <c r="F40" s="41"/>
+      <c r="G40" s="137"/>
+      <c r="H40" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="J40" s="103"/>
+      <c r="K40" s="103"/>
+      <c r="L40" s="103"/>
+      <c r="M40" s="103"/>
+      <c r="N40" s="103"/>
+    </row>
+    <row r="41" spans="1:14" s="124" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="123"/>
+      <c r="B41" s="135" t="s">
         <v>139</v>
       </c>
-      <c r="C40" s="136"/>
-      <c r="D40" s="126"/>
-      <c r="E40" s="127"/>
-      <c r="F40" s="127"/>
-      <c r="G40" s="138"/>
-      <c r="H40" s="129"/>
-      <c r="J40" s="125"/>
-      <c r="K40" s="125"/>
-      <c r="L40" s="125"/>
-      <c r="M40" s="125"/>
-      <c r="N40" s="125"/>
-    </row>
-    <row r="41" spans="1:14" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="99"/>
-      <c r="B41" s="92"/>
-      <c r="C41" s="41" t="s">
-        <v>138</v>
-      </c>
-      <c r="D41" s="94" t="s">
-        <v>117</v>
-      </c>
-      <c r="E41" s="94" t="s">
-        <v>141</v>
-      </c>
-      <c r="F41" s="41"/>
-      <c r="G41" s="137"/>
-      <c r="H41" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="J41" s="103"/>
-      <c r="K41" s="103"/>
-      <c r="L41" s="103"/>
-      <c r="M41" s="103"/>
-      <c r="N41" s="103"/>
+      <c r="C41" s="136"/>
+      <c r="D41" s="126"/>
+      <c r="E41" s="127"/>
+      <c r="F41" s="127"/>
+      <c r="G41" s="138"/>
+      <c r="H41" s="129"/>
+      <c r="J41" s="125"/>
+      <c r="K41" s="125"/>
+      <c r="L41" s="125"/>
+      <c r="M41" s="125"/>
+      <c r="N41" s="125"/>
     </row>
     <row r="42" spans="1:14" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="99"/>
       <c r="B42" s="92"/>
       <c r="C42" s="41" t="s">
-        <v>171</v>
+        <v>138</v>
       </c>
       <c r="D42" s="94" t="s">
         <v>117</v>
       </c>
       <c r="E42" s="94" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F42" s="41"/>
       <c r="G42" s="137"/>
@@ -34661,57 +34667,57 @@
       <c r="M42" s="103"/>
       <c r="N42" s="103"/>
     </row>
-    <row r="43" spans="1:14" s="124" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="123"/>
-      <c r="B43" s="135" t="s">
+    <row r="43" spans="1:14" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="99"/>
+      <c r="B43" s="92"/>
+      <c r="C43" s="41" t="s">
+        <v>171</v>
+      </c>
+      <c r="D43" s="94" t="s">
+        <v>117</v>
+      </c>
+      <c r="E43" s="94" t="s">
+        <v>140</v>
+      </c>
+      <c r="F43" s="41"/>
+      <c r="G43" s="137"/>
+      <c r="H43" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="J43" s="103"/>
+      <c r="K43" s="103"/>
+      <c r="L43" s="103"/>
+      <c r="M43" s="103"/>
+      <c r="N43" s="103"/>
+    </row>
+    <row r="44" spans="1:14" s="124" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="123"/>
+      <c r="B44" s="135" t="s">
         <v>165</v>
       </c>
-      <c r="C43" s="136"/>
-      <c r="D43" s="126"/>
-      <c r="E43" s="127"/>
-      <c r="F43" s="127"/>
-      <c r="G43" s="138"/>
-      <c r="H43" s="129"/>
-      <c r="J43" s="125"/>
-      <c r="K43" s="125"/>
-      <c r="L43" s="125"/>
-      <c r="M43" s="125"/>
-      <c r="N43" s="125"/>
-    </row>
-    <row r="44" spans="1:14" s="37" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="99"/>
-      <c r="B44" s="92"/>
-      <c r="C44" s="41" t="s">
-        <v>146</v>
-      </c>
-      <c r="D44" s="94" t="s">
-        <v>99</v>
-      </c>
-      <c r="E44" s="94" t="s">
-        <v>145</v>
-      </c>
-      <c r="F44" s="41"/>
-      <c r="G44" s="137"/>
-      <c r="H44" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="J44" s="103"/>
-      <c r="K44" s="103"/>
-      <c r="L44" s="103"/>
-      <c r="M44" s="103"/>
-      <c r="N44" s="103"/>
-    </row>
-    <row r="45" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C44" s="136"/>
+      <c r="D44" s="126"/>
+      <c r="E44" s="127"/>
+      <c r="F44" s="127"/>
+      <c r="G44" s="138"/>
+      <c r="H44" s="129"/>
+      <c r="J44" s="125"/>
+      <c r="K44" s="125"/>
+      <c r="L44" s="125"/>
+      <c r="M44" s="125"/>
+      <c r="N44" s="125"/>
+    </row>
+    <row r="45" spans="1:14" s="37" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A45" s="99"/>
       <c r="B45" s="92"/>
       <c r="C45" s="41" t="s">
-        <v>34</v>
+        <v>146</v>
       </c>
       <c r="D45" s="94" t="s">
         <v>99</v>
       </c>
       <c r="E45" s="94" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="F45" s="41"/>
       <c r="G45" s="137"/>
@@ -34728,13 +34734,13 @@
       <c r="A46" s="99"/>
       <c r="B46" s="92"/>
       <c r="C46" s="41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D46" s="94" t="s">
         <v>99</v>
       </c>
       <c r="E46" s="94" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F46" s="41"/>
       <c r="G46" s="137"/>
@@ -34751,13 +34757,13 @@
       <c r="A47" s="99"/>
       <c r="B47" s="92"/>
       <c r="C47" s="41" t="s">
-        <v>155</v>
+        <v>35</v>
       </c>
       <c r="D47" s="94" t="s">
         <v>99</v>
       </c>
       <c r="E47" s="94" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F47" s="41"/>
       <c r="G47" s="137"/>
@@ -34770,17 +34776,17 @@
       <c r="M47" s="103"/>
       <c r="N47" s="103"/>
     </row>
-    <row r="48" spans="1:14" s="37" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="100"/>
+    <row r="48" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="99"/>
       <c r="B48" s="92"/>
       <c r="C48" s="41" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="D48" s="94" t="s">
         <v>99</v>
       </c>
       <c r="E48" s="94" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="F48" s="41"/>
       <c r="G48" s="137"/>
@@ -34793,17 +34799,17 @@
       <c r="M48" s="103"/>
       <c r="N48" s="103"/>
     </row>
-    <row r="49" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" s="37" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A49" s="100"/>
       <c r="B49" s="92"/>
       <c r="C49" s="41" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="D49" s="94" t="s">
         <v>99</v>
       </c>
       <c r="E49" s="94" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="F49" s="41"/>
       <c r="G49" s="137"/>
@@ -34820,11 +34826,13 @@
       <c r="A50" s="100"/>
       <c r="B50" s="92"/>
       <c r="C50" s="41" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
-      <c r="D50" s="94"/>
+      <c r="D50" s="94" t="s">
+        <v>99</v>
+      </c>
       <c r="E50" s="94" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F50" s="41"/>
       <c r="G50" s="137"/>
@@ -34837,17 +34845,15 @@
       <c r="M50" s="103"/>
       <c r="N50" s="103"/>
     </row>
-    <row r="51" spans="1:14" s="37" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="100"/>
       <c r="B51" s="92"/>
       <c r="C51" s="41" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
-      <c r="D51" s="94" t="s">
-        <v>99</v>
-      </c>
+      <c r="D51" s="94"/>
       <c r="E51" s="94" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="F51" s="41"/>
       <c r="G51" s="137"/>
@@ -34860,20 +34866,20 @@
       <c r="M51" s="103"/>
       <c r="N51" s="103"/>
     </row>
-    <row r="52" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" s="37" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A52" s="100"/>
       <c r="B52" s="92"/>
-      <c r="C52" s="141" t="s">
-        <v>49</v>
+      <c r="C52" s="41" t="s">
+        <v>169</v>
       </c>
       <c r="D52" s="94" t="s">
         <v>99</v>
       </c>
-      <c r="E52" s="142" t="s">
-        <v>181</v>
+      <c r="E52" s="94" t="s">
+        <v>180</v>
       </c>
-      <c r="F52" s="141"/>
-      <c r="G52" s="143"/>
+      <c r="F52" s="41"/>
+      <c r="G52" s="137"/>
       <c r="H52" s="42" t="s">
         <v>46</v>
       </c>
@@ -34887,12 +34893,14 @@
       <c r="A53" s="100"/>
       <c r="B53" s="92"/>
       <c r="C53" s="141" t="s">
-        <v>178</v>
+        <v>49</v>
       </c>
       <c r="D53" s="94" t="s">
         <v>99</v>
       </c>
-      <c r="E53" s="142"/>
+      <c r="E53" s="142" t="s">
+        <v>181</v>
+      </c>
       <c r="F53" s="141"/>
       <c r="G53" s="143"/>
       <c r="H53" s="42" t="s">
@@ -34906,17 +34914,17 @@
     </row>
     <row r="54" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="100"/>
-      <c r="B54" s="93"/>
-      <c r="C54" s="44" t="s">
-        <v>172</v>
+      <c r="B54" s="92"/>
+      <c r="C54" s="141" t="s">
+        <v>178</v>
       </c>
-      <c r="D54" s="95" t="s">
+      <c r="D54" s="94" t="s">
         <v>99</v>
       </c>
-      <c r="E54" s="95"/>
-      <c r="F54" s="44"/>
-      <c r="G54" s="139"/>
-      <c r="H54" s="45" t="s">
+      <c r="E54" s="142"/>
+      <c r="F54" s="141"/>
+      <c r="G54" s="143"/>
+      <c r="H54" s="42" t="s">
         <v>46</v>
       </c>
       <c r="J54" s="103"/>
@@ -34927,13 +34935,19 @@
     </row>
     <row r="55" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="100"/>
-      <c r="B55" s="117"/>
-      <c r="C55" s="36"/>
-      <c r="D55" s="106"/>
-      <c r="E55" s="36"/>
-      <c r="F55" s="36"/>
-      <c r="G55" s="43"/>
-      <c r="H55" s="43"/>
+      <c r="B55" s="93"/>
+      <c r="C55" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="D55" s="95" t="s">
+        <v>99</v>
+      </c>
+      <c r="E55" s="95"/>
+      <c r="F55" s="44"/>
+      <c r="G55" s="139"/>
+      <c r="H55" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="J55" s="103"/>
       <c r="K55" s="103"/>
       <c r="L55" s="103"/>
@@ -34948,11 +34962,12 @@
       <c r="E56" s="36"/>
       <c r="F56" s="36"/>
       <c r="G56" s="43"/>
-      <c r="I56" s="103"/>
+      <c r="H56" s="43"/>
       <c r="J56" s="103"/>
       <c r="K56" s="103"/>
       <c r="L56" s="103"/>
       <c r="M56" s="103"/>
+      <c r="N56" s="103"/>
     </row>
     <row r="57" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="100"/>
@@ -35010,11 +35025,9 @@
       <c r="L60" s="103"/>
       <c r="M60" s="103"/>
     </row>
-    <row r="61" spans="1:14" s="37" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="100"/>
-      <c r="B61" s="118" t="s">
-        <v>51</v>
-      </c>
+      <c r="B61" s="117"/>
       <c r="C61" s="36"/>
       <c r="D61" s="106"/>
       <c r="E61" s="36"/>
@@ -35026,13 +35039,15 @@
       <c r="L61" s="103"/>
       <c r="M61" s="103"/>
     </row>
-    <row r="62" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" s="37" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A62" s="100"/>
-      <c r="B62" s="20"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="101"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
+      <c r="B62" s="118" t="s">
+        <v>51</v>
+      </c>
+      <c r="C62" s="36"/>
+      <c r="D62" s="106"/>
+      <c r="E62" s="36"/>
+      <c r="F62" s="36"/>
       <c r="G62" s="43"/>
       <c r="I62" s="103"/>
       <c r="J62" s="103"/>
@@ -35042,19 +35057,11 @@
     </row>
     <row r="63" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="100"/>
-      <c r="B63" s="119" t="s">
-        <v>33</v>
-      </c>
-      <c r="C63" s="52" t="s">
-        <v>52</v>
-      </c>
-      <c r="D63" s="107"/>
-      <c r="E63" s="52" t="s">
-        <v>53</v>
-      </c>
-      <c r="F63" s="53" t="s">
-        <v>54</v>
-      </c>
+      <c r="B63" s="20"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="101"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
       <c r="G63" s="43"/>
       <c r="I63" s="103"/>
       <c r="J63" s="103"/>
@@ -35064,18 +35071,18 @@
     </row>
     <row r="64" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="100"/>
-      <c r="B64" s="91" t="s">
-        <v>55</v>
+      <c r="B64" s="119" t="s">
+        <v>33</v>
       </c>
-      <c r="C64" s="46" t="s">
-        <v>56</v>
+      <c r="C64" s="52" t="s">
+        <v>52</v>
       </c>
-      <c r="D64" s="108"/>
-      <c r="E64" s="46" t="s">
-        <v>57</v>
+      <c r="D64" s="107"/>
+      <c r="E64" s="52" t="s">
+        <v>53</v>
       </c>
-      <c r="F64" s="47" t="s">
-        <v>58</v>
+      <c r="F64" s="53" t="s">
+        <v>54</v>
       </c>
       <c r="G64" s="43"/>
       <c r="I64" s="103"/>
@@ -35086,13 +35093,19 @@
     </row>
     <row r="65" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="100"/>
-      <c r="B65" s="92"/>
-      <c r="C65" s="48" t="s">
-        <v>59</v>
+      <c r="B65" s="91" t="s">
+        <v>55</v>
       </c>
-      <c r="D65" s="109"/>
-      <c r="E65" s="48"/>
-      <c r="F65" s="49"/>
+      <c r="C65" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="D65" s="108"/>
+      <c r="E65" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="F65" s="47" t="s">
+        <v>58</v>
+      </c>
       <c r="G65" s="43"/>
       <c r="I65" s="103"/>
       <c r="J65" s="103"/>
@@ -35104,13 +35117,11 @@
       <c r="A66" s="100"/>
       <c r="B66" s="92"/>
       <c r="C66" s="48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D66" s="109"/>
       <c r="E66" s="48"/>
-      <c r="F66" s="49" t="s">
-        <v>61</v>
-      </c>
+      <c r="F66" s="49"/>
       <c r="G66" s="43"/>
       <c r="I66" s="103"/>
       <c r="J66" s="103"/>
@@ -35122,12 +35133,12 @@
       <c r="A67" s="100"/>
       <c r="B67" s="92"/>
       <c r="C67" s="48" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D67" s="109"/>
       <c r="E67" s="48"/>
       <c r="F67" s="49" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G67" s="43"/>
       <c r="I67" s="103"/>
@@ -35138,13 +35149,15 @@
     </row>
     <row r="68" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="100"/>
-      <c r="B68" s="93"/>
-      <c r="C68" s="54" t="s">
-        <v>64</v>
+      <c r="B68" s="92"/>
+      <c r="C68" s="48" t="s">
+        <v>62</v>
       </c>
-      <c r="D68" s="110"/>
-      <c r="E68" s="54"/>
-      <c r="F68" s="55"/>
+      <c r="D68" s="109"/>
+      <c r="E68" s="48"/>
+      <c r="F68" s="49" t="s">
+        <v>63</v>
+      </c>
       <c r="G68" s="43"/>
       <c r="I68" s="103"/>
       <c r="J68" s="103"/>
@@ -35152,21 +35165,15 @@
       <c r="L68" s="103"/>
       <c r="M68" s="103"/>
     </row>
-    <row r="69" spans="1:13" s="37" customFormat="1" ht="42" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="100"/>
-      <c r="B69" s="89" t="s">
-        <v>65</v>
+      <c r="B69" s="93"/>
+      <c r="C69" s="54" t="s">
+        <v>64</v>
       </c>
-      <c r="C69" s="61" t="s">
-        <v>66</v>
-      </c>
-      <c r="D69" s="111"/>
-      <c r="E69" s="61" t="s">
-        <v>67</v>
-      </c>
-      <c r="F69" s="68" t="s">
-        <v>85</v>
-      </c>
+      <c r="D69" s="110"/>
+      <c r="E69" s="54"/>
+      <c r="F69" s="55"/>
       <c r="G69" s="43"/>
       <c r="I69" s="103"/>
       <c r="J69" s="103"/>
@@ -35174,18 +35181,20 @@
       <c r="L69" s="103"/>
       <c r="M69" s="103"/>
     </row>
-    <row r="70" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" s="37" customFormat="1" ht="42" x14ac:dyDescent="0.25">
       <c r="A70" s="100"/>
-      <c r="B70" s="90"/>
-      <c r="C70" s="62" t="s">
-        <v>68</v>
+      <c r="B70" s="89" t="s">
+        <v>65</v>
       </c>
-      <c r="D70" s="112"/>
-      <c r="E70" s="62" t="s">
-        <v>68</v>
+      <c r="C70" s="61" t="s">
+        <v>66</v>
       </c>
-      <c r="F70" s="63" t="s">
-        <v>69</v>
+      <c r="D70" s="111"/>
+      <c r="E70" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="F70" s="68" t="s">
+        <v>85</v>
       </c>
       <c r="G70" s="43"/>
       <c r="I70" s="103"/>
@@ -35196,18 +35205,16 @@
     </row>
     <row r="71" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="100"/>
-      <c r="B71" s="91" t="s">
-        <v>70</v>
+      <c r="B71" s="90"/>
+      <c r="C71" s="62" t="s">
+        <v>68</v>
       </c>
-      <c r="C71" s="58" t="s">
-        <v>71</v>
+      <c r="D71" s="112"/>
+      <c r="E71" s="62" t="s">
+        <v>68</v>
       </c>
-      <c r="D71" s="113"/>
-      <c r="E71" s="58" t="s">
-        <v>72</v>
-      </c>
-      <c r="F71" s="59" t="s">
-        <v>73</v>
+      <c r="F71" s="63" t="s">
+        <v>69</v>
       </c>
       <c r="G71" s="43"/>
       <c r="I71" s="103"/>
@@ -35218,14 +35225,18 @@
     </row>
     <row r="72" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="100"/>
-      <c r="B72" s="93"/>
-      <c r="C72" s="54"/>
-      <c r="D72" s="110"/>
-      <c r="E72" s="56" t="s">
-        <v>74</v>
+      <c r="B72" s="91" t="s">
+        <v>70</v>
       </c>
-      <c r="F72" s="57" t="s">
-        <v>75</v>
+      <c r="C72" s="58" t="s">
+        <v>71</v>
+      </c>
+      <c r="D72" s="113"/>
+      <c r="E72" s="58" t="s">
+        <v>72</v>
+      </c>
+      <c r="F72" s="59" t="s">
+        <v>73</v>
       </c>
       <c r="G72" s="43"/>
       <c r="I72" s="103"/>
@@ -35236,18 +35247,14 @@
     </row>
     <row r="73" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="100"/>
-      <c r="B73" s="67" t="s">
-        <v>76</v>
+      <c r="B73" s="93"/>
+      <c r="C73" s="54"/>
+      <c r="D73" s="110"/>
+      <c r="E73" s="56" t="s">
+        <v>74</v>
       </c>
-      <c r="C73" s="64" t="s">
-        <v>77</v>
-      </c>
-      <c r="D73" s="114"/>
-      <c r="E73" s="65">
-        <v>2013</v>
-      </c>
-      <c r="F73" s="66" t="s">
-        <v>78</v>
+      <c r="F73" s="57" t="s">
+        <v>75</v>
       </c>
       <c r="G73" s="43"/>
       <c r="I73" s="103"/>
@@ -35258,18 +35265,18 @@
     </row>
     <row r="74" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="100"/>
-      <c r="B74" s="91" t="s">
-        <v>79</v>
+      <c r="B74" s="67" t="s">
+        <v>76</v>
       </c>
-      <c r="C74" s="46" t="s">
-        <v>80</v>
+      <c r="C74" s="64" t="s">
+        <v>77</v>
       </c>
-      <c r="D74" s="108"/>
-      <c r="E74" s="46" t="s">
-        <v>81</v>
+      <c r="D74" s="114"/>
+      <c r="E74" s="65">
+        <v>2013</v>
       </c>
-      <c r="F74" s="47" t="s">
-        <v>82</v>
+      <c r="F74" s="66" t="s">
+        <v>78</v>
       </c>
       <c r="G74" s="43"/>
       <c r="I74" s="103"/>
@@ -35278,18 +35285,20 @@
       <c r="L74" s="103"/>
       <c r="M74" s="103"/>
     </row>
-    <row r="75" spans="1:13" s="37" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="100"/>
-      <c r="B75" s="92"/>
-      <c r="C75" s="48" t="s">
-        <v>83</v>
+      <c r="B75" s="91" t="s">
+        <v>79</v>
       </c>
-      <c r="D75" s="109"/>
-      <c r="E75" s="48" t="s">
-        <v>83</v>
+      <c r="C75" s="46" t="s">
+        <v>80</v>
       </c>
-      <c r="F75" s="50" t="s">
-        <v>86</v>
+      <c r="D75" s="108"/>
+      <c r="E75" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="F75" s="47" t="s">
+        <v>82</v>
       </c>
       <c r="G75" s="43"/>
       <c r="I75" s="103"/>
@@ -35298,15 +35307,19 @@
       <c r="L75" s="103"/>
       <c r="M75" s="103"/>
     </row>
-    <row r="76" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" s="37" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A76" s="100"/>
       <c r="B76" s="92"/>
       <c r="C76" s="48" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D76" s="109"/>
-      <c r="E76" s="48"/>
-      <c r="F76" s="49"/>
+      <c r="E76" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="F76" s="50" t="s">
+        <v>86</v>
+      </c>
       <c r="G76" s="43"/>
       <c r="I76" s="103"/>
       <c r="J76" s="103"/>
@@ -35314,17 +35327,15 @@
       <c r="L76" s="103"/>
       <c r="M76" s="103"/>
     </row>
-    <row r="77" spans="1:13" s="37" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="100"/>
-      <c r="B77" s="93"/>
-      <c r="C77" s="60" t="s">
-        <v>68</v>
+      <c r="B77" s="92"/>
+      <c r="C77" s="48" t="s">
+        <v>84</v>
       </c>
-      <c r="D77" s="115"/>
-      <c r="E77" s="60"/>
-      <c r="F77" s="51" t="s">
-        <v>87</v>
-      </c>
+      <c r="D77" s="109"/>
+      <c r="E77" s="48"/>
+      <c r="F77" s="49"/>
       <c r="G77" s="43"/>
       <c r="I77" s="103"/>
       <c r="J77" s="103"/>
@@ -35332,13 +35343,17 @@
       <c r="L77" s="103"/>
       <c r="M77" s="103"/>
     </row>
-    <row r="78" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" s="37" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A78" s="100"/>
-      <c r="B78" s="117"/>
-      <c r="C78" s="36"/>
-      <c r="D78" s="106"/>
-      <c r="E78" s="36"/>
-      <c r="F78" s="36"/>
+      <c r="B78" s="93"/>
+      <c r="C78" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="D78" s="115"/>
+      <c r="E78" s="60"/>
+      <c r="F78" s="51" t="s">
+        <v>87</v>
+      </c>
       <c r="G78" s="43"/>
       <c r="I78" s="103"/>
       <c r="J78" s="103"/>
@@ -36312,19 +36327,19 @@
       <c r="L147" s="103"/>
       <c r="M147" s="103"/>
     </row>
-    <row r="148" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="97"/>
+    <row r="148" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="100"/>
       <c r="B148" s="117"/>
-      <c r="C148" s="1"/>
-      <c r="D148" s="101"/>
-      <c r="E148" s="1"/>
-      <c r="F148" s="1"/>
-      <c r="G148" s="39"/>
-      <c r="I148" s="102"/>
-      <c r="J148" s="102"/>
-      <c r="K148" s="102"/>
-      <c r="L148" s="102"/>
-      <c r="M148" s="102"/>
+      <c r="C148" s="36"/>
+      <c r="D148" s="106"/>
+      <c r="E148" s="36"/>
+      <c r="F148" s="36"/>
+      <c r="G148" s="43"/>
+      <c r="I148" s="103"/>
+      <c r="J148" s="103"/>
+      <c r="K148" s="103"/>
+      <c r="L148" s="103"/>
+      <c r="M148" s="103"/>
     </row>
     <row r="149" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="97"/>
@@ -37992,10 +38007,19 @@
       <c r="L267" s="102"/>
       <c r="M267" s="102"/>
     </row>
-    <row r="268" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H268" s="1"/>
-      <c r="I268" s="101"/>
-      <c r="N268" s="1"/>
+    <row r="268" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A268" s="97"/>
+      <c r="B268" s="117"/>
+      <c r="C268" s="1"/>
+      <c r="D268" s="101"/>
+      <c r="E268" s="1"/>
+      <c r="F268" s="1"/>
+      <c r="G268" s="39"/>
+      <c r="I268" s="102"/>
+      <c r="J268" s="102"/>
+      <c r="K268" s="102"/>
+      <c r="L268" s="102"/>
+      <c r="M268" s="102"/>
     </row>
     <row r="269" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H269" s="1"/>
@@ -42272,8 +42296,13 @@
       <c r="I1123" s="101"/>
       <c r="N1123" s="1"/>
     </row>
+    <row r="1124" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H1124" s="1"/>
+      <c r="I1124" s="101"/>
+      <c r="N1124" s="1"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="H11:H14 H41:H42 H44:H48 H9 H24:H30 H32:H35 H16:H22">
+  <conditionalFormatting sqref="H11:H14 H42:H43 H45:H49 H9 H33:H36 H16:H22 H24:H31">
     <cfRule type="cellIs" dxfId="13" priority="45" operator="equal">
       <formula>$A$11</formula>
     </cfRule>
@@ -42281,7 +42310,7 @@
       <formula>$A$7</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H50:H53">
+  <conditionalFormatting sqref="H51:H54">
     <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
       <formula>$A$11</formula>
     </cfRule>
@@ -42289,7 +42318,7 @@
       <formula>$A$7</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H49">
+  <conditionalFormatting sqref="H50">
     <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
       <formula>$A$11</formula>
     </cfRule>
@@ -42297,7 +42326,7 @@
       <formula>$A$7</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H37">
+  <conditionalFormatting sqref="H38">
     <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
       <formula>$A$11</formula>
     </cfRule>
@@ -42305,7 +42334,7 @@
       <formula>$A$7</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H38:H39">
+  <conditionalFormatting sqref="H39:H40">
     <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
       <formula>$A$11</formula>
     </cfRule>
@@ -42313,7 +42342,7 @@
       <formula>$A$7</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
+  <conditionalFormatting sqref="H36">
     <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>$A$11</formula>
     </cfRule>
@@ -42321,7 +42350,7 @@
       <formula>$A$7</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H54">
+  <conditionalFormatting sqref="H55">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>$A$11</formula>
     </cfRule>
@@ -42330,10 +42359,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H9 H11:H54" xr:uid="{38080977-4269-4EAA-AF58-F25EAE9C07B6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H9 H11:H55" xr:uid="{38080977-4269-4EAA-AF58-F25EAE9C07B6}">
       <formula1>$L$7:$L$8</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:D9 D11:D54" xr:uid="{3B8CE9F0-680B-4E0A-B694-A1F2EA07B84E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:D9 D11:D55" xr:uid="{3B8CE9F0-680B-4E0A-B694-A1F2EA07B84E}">
       <formula1>$J$7:$J$10</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>